<commit_message>
Recorded performance of commits
</commit_message>
<xml_diff>
--- a/Algorithm.CSharp/Benchmarks/EmptyMinute400EquityAlgorithm.xlsx
+++ b/Algorithm.CSharp/Benchmarks/EmptyMinute400EquityAlgorithm.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>dc1e83a</t>
   </si>
@@ -40,6 +40,21 @@
   </si>
   <si>
     <t>Use ParallelRunner with ProcessorCount-3 threads in FileSystemDataFeeed</t>
+  </si>
+  <si>
+    <t>Change thread count setting</t>
+  </si>
+  <si>
+    <t>1e8b92d</t>
+  </si>
+  <si>
+    <t>a88d2af</t>
+  </si>
+  <si>
+    <t>Make Slice DataDictionary lazy eval</t>
+  </si>
+  <si>
+    <t>Make algo run on dedicated thread</t>
   </si>
 </sst>
 </file>
@@ -378,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,6 +449,45 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>19.16</v>
+      </c>
+      <c r="C4">
+        <v>186</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>18.37</v>
+      </c>
+      <c r="C5">
+        <v>195</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>18.3</v>
+      </c>
+      <c r="C6">
+        <v>196</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>